<commit_message>
Results with RF predictions: combined and 2019-only
</commit_message>
<xml_diff>
--- a/R_Logit_Models/SMTO_Combined/SMTO_Combined_Results.xlsx
+++ b/R_Logit_Models/SMTO_Combined/SMTO_Combined_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\Ethan\TMG\Research\PORPOS-TMG\R_Logit_Models\SMTO_Combined\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8C07FB-3EE0-4F27-A5F0-427DDB8567AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC17AD1D-6609-4FC9-BB89-BF8D0873BBE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Model</t>
   </si>
@@ -51,10 +51,46 @@
     <t>Log Likelihood</t>
   </si>
   <si>
-    <t>Combined</t>
-  </si>
-  <si>
-    <t>Combined + Closest</t>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>Ref + Closest</t>
+  </si>
+  <si>
+    <t>Col Prob</t>
+  </si>
+  <si>
+    <t>Uni Prob</t>
+  </si>
+  <si>
+    <t>Pred Type</t>
+  </si>
+  <si>
+    <t>Both Prob</t>
+  </si>
+  <si>
+    <t>Col Prob + Closest</t>
+  </si>
+  <si>
+    <t>Uni Prob + Closest</t>
+  </si>
+  <si>
+    <t>Pred Type + Closest</t>
+  </si>
+  <si>
+    <t>Both Prob + Closest</t>
+  </si>
+  <si>
+    <t>Prob Col</t>
+  </si>
+  <si>
+    <t>Prob Uni</t>
+  </si>
+  <si>
+    <t>Prob Type</t>
+  </si>
+  <si>
+    <t>Prob Type + Closest</t>
   </si>
 </sst>
 </file>
@@ -65,7 +101,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +120,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,7 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,12 +166,27 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -226,17 +283,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DA9DCFD-F99F-40BB-90A8-F2B7B5586713}" name="Table2" displayName="Table2" ref="A1:H3" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:H3" xr:uid="{2BC126AE-02B1-452B-AEA6-BB1370364F81}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DA9DCFD-F99F-40BB-90A8-F2B7B5586713}" name="Table2" displayName="Table2" ref="A1:K13" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:K13" xr:uid="{2BC126AE-02B1-452B-AEA6-BB1370364F81}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{2A3D203E-4EBA-460C-8667-BC7E2C726538}" name="Model"/>
-    <tableColumn id="2" xr3:uid="{9A89F7CA-D1F2-4F8B-B0B0-BE5F9B9B0C00}" name="B_DIST" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{DD51AAE0-EEB7-4011-9AFA-92269975C53C}" name="B_ENROL" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{F31773E2-CB7B-47EA-B8A6-CD8C21614155}" name="B_CLOSEST" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{F578ED18-2145-4D33-9F0B-D4BFB8397756}" name="B_FAM_DIST" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{0BA8D3E4-EA20-4F8B-8F4A-2AD984506ED4}" name="Hardmax Acc" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{7D9100EC-E322-460C-AE70-3BD18DEEB87B}" name="Softmax APO" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="8" xr3:uid="{0E6E2BF7-388B-4B59-B5CD-C665BA5DF8F7}" name="Log Likelihood" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{9A89F7CA-D1F2-4F8B-B0B0-BE5F9B9B0C00}" name="B_DIST" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{DD51AAE0-EEB7-4011-9AFA-92269975C53C}" name="B_ENROL" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{F31773E2-CB7B-47EA-B8A6-CD8C21614155}" name="B_CLOSEST" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{F578ED18-2145-4D33-9F0B-D4BFB8397756}" name="B_FAM_DIST" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{FCA96AF9-570B-4A7E-93AB-B9F398A17DF6}" name="Prob Col" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{982AB95E-F6FB-4391-B323-9E28B0030484}" name="Prob Uni" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{CC08F85B-FD41-4399-9F12-D4E75A99A6CC}" name="Pred Type" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{0BA8D3E4-EA20-4F8B-8F4A-2AD984506ED4}" name="Hardmax Acc" dataDxfId="5" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{7D9100EC-E322-460C-AE70-3BD18DEEB87B}" name="Softmax APO" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{0E6E2BF7-388B-4B59-B5CD-C665BA5DF8F7}" name="Log Likelihood" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -505,19 +565,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="16.54296875" customWidth="1"/>
+    <col min="2" max="11" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,16 +594,25 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -557,43 +626,466 @@
       <c r="E2" s="2">
         <v>3.7806199999999998E-2</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3">
         <v>0.40917599999999998</v>
       </c>
-      <c r="G2" s="3">
+      <c r="J2" s="3">
         <v>0.26787260000000002</v>
       </c>
-      <c r="H2" s="4">
+      <c r="K2" s="4">
         <v>-55263.65</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-8.7949440000000004E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.1452232499999999</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>3.3344400000000003E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.0542205999999998</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="3">
+        <v>0.42317870000000002</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.27647369999999999</v>
+      </c>
+      <c r="K3" s="4">
+        <v>-54524.53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-9.2299939999999997E-2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.78988632000000003</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>3.5135899999999998E-2</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <v>1.80802851</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3">
+        <v>0.40549780000000002</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.2762097</v>
+      </c>
+      <c r="K4" s="4">
+        <v>-52948.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-8.7632450000000001E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.86637257000000001</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>3.1362889999999997E-2</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <v>1.6228740399999999</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.42372720000000003</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.28719749999999999</v>
+      </c>
+      <c r="K5" s="4">
+        <v>-52084.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-8.7523340000000005E-2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.79693468999999995</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>3.0889409999999999E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.65252899</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2.65252899</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3">
+        <v>0.42779250000000002</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.28761589999999998</v>
+      </c>
+      <c r="K6" s="4">
+        <v>-51414.61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-8.5885359999999994E-2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.83173856000000002</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>2.9717110000000001E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3.6776201099999999</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2.5234539100000002</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="3">
+        <v>0.42669550000000001</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.2897979</v>
+      </c>
+      <c r="K7" s="4">
+        <v>-51258.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B8" s="2">
         <v>-8.1441009999999994E-2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C8" s="2">
         <v>1.06716554</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D8" s="2">
         <v>1.1660405300000001</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E8" s="2">
         <v>2.729786E-2</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3">
         <v>0.40185199999999999</v>
       </c>
-      <c r="G3" s="3">
+      <c r="J8" s="3">
         <v>0.28476639999999998</v>
       </c>
-      <c r="H3" s="4">
+      <c r="K8" s="4">
         <v>-54354.96</v>
       </c>
     </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-7.608827E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.1467958899999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.16594687</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.3207559999999999E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2.0547677800000002</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="3">
+        <v>0.41382200000000002</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.2930043</v>
+      </c>
+      <c r="K9" s="4">
+        <v>-53640.69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-8.0270300000000003E-2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.79116507999999997</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.14798018</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.454284E-2</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>1.8156287600000001</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3">
+        <v>0.40240049999999999</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.29257369999999999</v>
+      </c>
+      <c r="K10" s="4">
+        <v>-52065.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2">
+        <v>-7.5902620000000004E-2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.79884573999999997</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.13125159</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.059629E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2.64901973</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2.64901973</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3">
+        <v>0.42146869999999997</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.30333189999999999</v>
+      </c>
+      <c r="K11" s="4">
+        <v>-50578.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2">
+        <v>-7.5961420000000002E-2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.86878783999999998</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.1395310400000001</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.113348E-2</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2">
+        <v>1.61851342</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.41979090000000002</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.30284280000000002</v>
+      </c>
+      <c r="K12" s="4">
+        <v>-51243.19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2">
+        <v>-7.4406990000000006E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.83330705999999999</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.1305202000000001</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.9576070000000001E-2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3.6544233899999998</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2.5225271999999999</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="5">
+        <v>0.42027490000000001</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.30539830000000001</v>
+      </c>
+      <c r="K13" s="4">
+        <v>-50429.93</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="I2:I13">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J13">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K13">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B13">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C13">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E13">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G13">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>